<commit_message>
added example users and codes to firebase
</commit_message>
<xml_diff>
--- a/doc/lists of species, usernames, and codes.xlsx
+++ b/doc/lists of species, usernames, and codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\CMPUT301Group\IHuntWithJavalins\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A69AB2-B636-4345-A696-85A17517EF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A69CD4-FA2E-45E9-AE99-904EBDFDABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
   </bookViews>
@@ -715,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -725,14 +725,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1405,14 +1403,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C971D1C0-66EE-4732-8814-024619477189}">
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
@@ -1426,7 +1424,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1484,7 +1482,7 @@
       <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="16" t="s">
         <v>63</v>
       </c>
       <c r="Q1" t="s">
@@ -1554,31 +1552,31 @@
       <c r="F3" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="P3" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="P3" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>445</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="11" t="s">
+      <c r="F4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="10" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1705,7 +1703,7 @@
       <c r="H9" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="16" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1881,7 +1879,7 @@
       <c r="J16" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="16" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2034,7 +2032,7 @@
       <c r="L22" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="P22" s="16" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2161,7 +2159,7 @@
       <c r="N27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="P27" s="18" t="s">
+      <c r="P27" s="16" t="s">
         <v>181</v>
       </c>
       <c r="U27" s="4" t="s">
@@ -2336,7 +2334,7 @@
         <f>E29+E30+E31+E32</f>
         <v>2550</v>
       </c>
-      <c r="P33" s="18">
+      <c r="P33" s="16">
         <f>E3+E9+E16+E22+E27</f>
         <v>2090</v>
       </c>
@@ -2417,7 +2415,7 @@
       <c r="O34" s="6">
         <v>5</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="17">
         <v>8</v>
       </c>
       <c r="Q34" s="6">
@@ -2488,7 +2486,7 @@
       <c r="O35">
         <v>4</v>
       </c>
-      <c r="P35" s="18">
+      <c r="P35" s="16">
         <v>5</v>
       </c>
       <c r="Q35">
@@ -2523,64 +2521,64 @@
       <c r="E36" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="13">
         <v>7</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>8</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <v>16</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="13">
         <v>14</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <v>15</v>
       </c>
-      <c r="K36" s="14">
+      <c r="K36" s="13">
         <v>17</v>
       </c>
-      <c r="L36" s="14">
+      <c r="L36" s="13">
         <v>18</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="13">
         <v>13</v>
       </c>
-      <c r="N36" s="14">
+      <c r="N36" s="13">
         <v>9</v>
       </c>
-      <c r="O36" s="14">
+      <c r="O36" s="13">
         <v>10</v>
       </c>
-      <c r="P36" s="19">
+      <c r="P36" s="17">
         <v>4</v>
       </c>
-      <c r="Q36" s="15">
+      <c r="Q36" s="14">
         <v>3</v>
       </c>
-      <c r="R36" s="15">
+      <c r="R36" s="14">
         <v>1</v>
       </c>
-      <c r="S36" s="15">
+      <c r="S36" s="14">
         <v>5</v>
       </c>
-      <c r="T36" s="15">
+      <c r="T36" s="14">
         <v>2</v>
       </c>
-      <c r="U36" s="15">
+      <c r="U36" s="14">
         <v>6</v>
       </c>
-      <c r="V36" s="16">
+      <c r="V36" s="6">
         <v>20</v>
       </c>
-      <c r="W36" s="16">
+      <c r="W36" s="6">
         <v>19</v>
       </c>
-      <c r="X36" s="14">
+      <c r="X36" s="13">
         <v>11</v>
       </c>
-      <c r="Y36" s="14">
+      <c r="Y36" s="13">
         <v>12</v>
       </c>
       <c r="Z36" t="s">
@@ -2591,10 +2589,10 @@
       <c r="E37" t="s">
         <v>185</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="9">
         <v>4168</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="9">
         <v>4168</v>
       </c>
       <c r="H37" s="4">
@@ -2615,22 +2613,22 @@
       <c r="M37">
         <v>712</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="10">
         <v>1753</v>
       </c>
-      <c r="O37" s="11">
+      <c r="O37" s="10">
         <v>1753</v>
       </c>
-      <c r="P37" s="18">
+      <c r="P37" s="16">
         <v>689</v>
       </c>
-      <c r="Q37" s="12">
+      <c r="Q37" s="11">
         <v>1356</v>
       </c>
-      <c r="R37" s="10">
+      <c r="R37" s="9">
         <v>4168</v>
       </c>
-      <c r="S37" s="13">
+      <c r="S37" s="12">
         <v>539</v>
       </c>
       <c r="T37">
@@ -2639,16 +2637,16 @@
       <c r="U37">
         <v>556</v>
       </c>
-      <c r="V37" s="9">
+      <c r="V37">
         <v>314</v>
       </c>
-      <c r="W37" s="13">
+      <c r="W37" s="12">
         <v>539</v>
       </c>
-      <c r="X37" s="11">
+      <c r="X37" s="10">
         <v>1753</v>
       </c>
-      <c r="Y37" s="12">
+      <c r="Y37" s="11">
         <v>1356</v>
       </c>
     </row>
@@ -2686,7 +2684,7 @@
       <c r="O38" s="6">
         <v>5</v>
       </c>
-      <c r="P38" s="19">
+      <c r="P38" s="17">
         <v>14</v>
       </c>
       <c r="Q38" s="6">
@@ -2704,10 +2702,10 @@
       <c r="U38" s="6">
         <v>15</v>
       </c>
-      <c r="V38" s="16">
+      <c r="V38" s="6">
         <v>19</v>
       </c>
-      <c r="W38" s="16">
+      <c r="W38" s="6">
         <v>17</v>
       </c>
       <c r="X38" s="6">

</xml_diff>

<commit_message>
brandon renamed xmls, activities; added generic photo attaching (no camera functionality for photos yet), made quick nav as homescreen, added viraj's delete dialog to code deletion feature, added viraj's scoreboard
</commit_message>
<xml_diff>
--- a/doc/lists of species, usernames, and codes.xlsx
+++ b/doc/lists of species, usernames, and codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\CMPUT301Group\IHuntWithJavalins\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A69CD4-FA2E-45E9-AE99-904EBDFDABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B3B9C6-4F17-4300-810D-4EC4C95EE59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="NamingConvention" sheetId="1" r:id="rId1"/>
@@ -1403,14 +1403,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C971D1C0-66EE-4732-8814-024619477189}">
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
made profile acitvity page that can query user's contact info and codes; codes can be analyzed to find total points, total codes, and highest code value
</commit_message>
<xml_diff>
--- a/doc/lists of species, usernames, and codes.xlsx
+++ b/doc/lists of species, usernames, and codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\CMPUT301Group\IHuntWithJavalins\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B3B9C6-4F17-4300-810D-4EC4C95EE59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A081E78-13BE-46B5-8374-DBF415DB620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
   </bookViews>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Original Merge with Brandon Branch
</commit_message>
<xml_diff>
--- a/doc/lists of species, usernames, and codes.xlsx
+++ b/doc/lists of species, usernames, and codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\CMPUT301Group\IHuntWithJavalins\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B3B9C6-4F17-4300-810D-4EC4C95EE59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A081E78-13BE-46B5-8374-DBF415DB620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
   </bookViews>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated scoreboard to use firebase (added firebase example users and codes)
</commit_message>
<xml_diff>
--- a/doc/lists of species, usernames, and codes.xlsx
+++ b/doc/lists of species, usernames, and codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\CMPUT301Group\IHuntWithJavalins\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponti\Desktop\Newfolder3\IHuntWithJavalins\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A081E78-13BE-46B5-8374-DBF415DB620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A1E67-A9AC-4905-A700-D4CF8CCB45AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{78FA460C-CDA3-406D-AEA8-1A2B16E90BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="NamingConvention" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="194">
   <si>
     <t>Fire</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>if equal, then most codes</t>
+  </si>
+  <si>
+    <t>Edmonton</t>
+  </si>
+  <si>
+    <t>Calgary</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1292,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,39 +1407,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C971D1C0-66EE-4732-8814-024619477189}">
-  <dimension ref="A1:AA38"/>
+  <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="73.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2718,6 +2725,68 @@
         <v>189</v>
       </c>
     </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H40" t="s">
+        <v>192</v>
+      </c>
+      <c r="I40" t="s">
+        <v>192</v>
+      </c>
+      <c r="J40" t="s">
+        <v>192</v>
+      </c>
+      <c r="K40" t="s">
+        <v>192</v>
+      </c>
+      <c r="L40" t="s">
+        <v>192</v>
+      </c>
+      <c r="M40" t="s">
+        <v>192</v>
+      </c>
+      <c r="N40" t="s">
+        <v>192</v>
+      </c>
+      <c r="O40" t="s">
+        <v>192</v>
+      </c>
+      <c r="P40" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>192</v>
+      </c>
+      <c r="R40" t="s">
+        <v>192</v>
+      </c>
+      <c r="S40" t="s">
+        <v>192</v>
+      </c>
+      <c r="T40" t="s">
+        <v>192</v>
+      </c>
+      <c r="U40" t="s">
+        <v>193</v>
+      </c>
+      <c r="V40" t="s">
+        <v>193</v>
+      </c>
+      <c r="W40" t="s">
+        <v>193</v>
+      </c>
+      <c r="X40" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>